<commit_message>
[woo] monster 테이블에 도감용  monster_desc 컬럼 추가
</commit_message>
<xml_diff>
--- a/Assets/Resource/ExcelData/monster.xlsx
+++ b/Assets/Resource/ExcelData/monster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\TextRPG\Assets\Resource\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE684BD-B47C-4E64-BA44-26874C2EED24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4F0678-3BD5-4FBA-925C-7337A9B9FBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15348" yWindow="7248" windowWidth="22368" windowHeight="11664" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="46296" windowHeight="25680" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="monster" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>int</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>img_wolf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monster_desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도감용 몬스터 설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검은빛이 도는 골렘입니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -609,9 +621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q15" sqref="Q15"/>
+      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
@@ -622,11 +634,11 @@
     <col min="12" max="12" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="14.5" style="3" customWidth="1"/>
     <col min="16" max="16" width="12" style="3" customWidth="1"/>
-    <col min="17" max="17" width="40" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="8.796875" style="3"/>
+    <col min="17" max="18" width="40" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" s="8" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -678,8 +690,11 @@
       <c r="Q1" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
+      <c r="R1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -731,8 +746,11 @@
       <c r="Q2" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -784,8 +802,11 @@
       <c r="Q3" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>10001</v>
       </c>
@@ -837,8 +858,11 @@
       <c r="Q4" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -853,8 +877,9 @@
       <c r="L5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -869,8 +894,9 @@
       <c r="L6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -885,8 +911,9 @@
       <c r="L7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -901,8 +928,9 @@
       <c r="L8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -917,8 +945,9 @@
       <c r="L9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -933,8 +962,9 @@
       <c r="L10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -949,8 +979,9 @@
       <c r="L11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -965,8 +996,9 @@
       <c r="L12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -981,8 +1013,9 @@
       <c r="L13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -997,8 +1030,9 @@
       <c r="L14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1013,8 +1047,9 @@
       <c r="L15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1029,6 +1064,7 @@
       <c r="L16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -1045,6 +1081,7 @@
       <c r="L17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
@@ -1061,6 +1098,7 @@
       <c r="L18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -1077,6 +1115,7 @@
       <c r="L19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>

</xml_diff>